<commit_message>
transient modeling, ecm edits
</commit_message>
<xml_diff>
--- a/FE12/Cell Modeling/FE11_P42A_EntropicCoefficients.xlsx
+++ b/FE12/Cell Modeling/FE11_P42A_EntropicCoefficients.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ad310da11adffc61/Documentos/GitHub/FE12-Accumulator/FE12/Cell Modeling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laptop\OneDrive - University of California, Davis\Documents\GitHub\FE12-Accumulator\FE12\Cell Modeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="128" documentId="13_ncr:1_{5390565A-ADB2-4860-8D55-CE8517E3BC43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{020D7028-379B-4525-B0A6-2C5695A73DF6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF942F4-F3B6-4ABA-BFD2-D9D93AABC278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{31AE9364-1268-41AB-B668-B2DC75F79138}"/>
+    <workbookView minimized="1" xWindow="4155" yWindow="4155" windowWidth="21600" windowHeight="12585" xr2:uid="{31AE9364-1268-41AB-B668-B2DC75F79138}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3646,8 +3646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DB795AD-713B-444C-8C0B-22AC1AA478F9}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13:J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>